<commit_message>
Tentatively completed wrangling for OLR using Subject:series to organize things
</commit_message>
<xml_diff>
--- a/amazonia/OLR/xls_standard_input_amazonia.xlsx
+++ b/amazonia/OLR/xls_standard_input_amazonia.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="756">
   <si>
     <t>text</t>
   </si>
@@ -2179,8 +2179,56 @@
 </t>
   </si>
   <si>
-    <t>Ca.1734
-Description from UNESCO:
+    <t xml:space="preserve">1616, (1623 Gurupá Fort Established)
+</t>
+  </si>
+  <si>
+    <t>1764, Jan. 02</t>
+  </si>
+  <si>
+    <t>1766</t>
+  </si>
+  <si>
+    <t>1697</t>
+  </si>
+  <si>
+    <t>1616</t>
+  </si>
+  <si>
+    <t>1734</t>
+  </si>
+  <si>
+    <t>ca. 1759</t>
+  </si>
+  <si>
+    <t>Ca. 1700s (likely)</t>
+  </si>
+  <si>
+    <t>1609, 1624</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>Ferreira, Alexandre Rodrigues, 1756-1815</t>
+  </si>
+  <si>
+    <t>Deavenport, James</t>
+  </si>
+  <si>
+    <t>Archivo General de la Nación de Colombia</t>
+  </si>
+  <si>
+    <t>Smith, Robert C.</t>
+  </si>
+  <si>
+    <t>Sweet, David Graham</t>
+  </si>
+  <si>
+    <t>UNESCO World Heritage Centre</t>
+  </si>
+  <si>
+    <t>Description from UNESCO:
 "The two structures, Fort Zeelandia and the Court of Policy Building are separated by about 10 minutes walk.
 The two should be considered together. The Fort itself was built circa 1743 whilst the Court Policy was built the same time- the latter is reputedly the oldest building in Guyana.
 (1) Fort Zeelandia 
@@ -2192,35 +2240,202 @@
 http://www.atlasofmutualheritage.nl/nl/Zeelandia-fort-Essequibo.255c</t>
   </si>
   <si>
-    <t xml:space="preserve">1616, (1623 Gurupá Fort Established)
-</t>
-  </si>
-  <si>
-    <t>1764, Jan. 02</t>
-  </si>
-  <si>
-    <t>1766</t>
-  </si>
-  <si>
-    <t>1697</t>
-  </si>
-  <si>
-    <t>1616</t>
-  </si>
-  <si>
-    <t>1734</t>
-  </si>
-  <si>
-    <t>ca. 1759</t>
-  </si>
-  <si>
-    <t>Ca. 1700s (likely)</t>
-  </si>
-  <si>
-    <t>1609, 1624</t>
-  </si>
-  <si>
-    <t>2016</t>
+    <t>1786</t>
+  </si>
+  <si>
+    <t>~ 1500 - 1800</t>
+  </si>
+  <si>
+    <t>1616-1776</t>
+  </si>
+  <si>
+    <t>Photographs Taken by James Deavenport, 2015</t>
+  </si>
+  <si>
+    <t>Fortification</t>
+  </si>
+  <si>
+    <t>Brazil--Belém</t>
+  </si>
+  <si>
+    <t>Brazil--Tabatinga (Amazonas)</t>
+  </si>
+  <si>
+    <t>South America--Guaporé River | Bolivia | Brazil</t>
+  </si>
+  <si>
+    <t>Fortification | Portuguese Colonial</t>
+  </si>
+  <si>
+    <t>Fortification | Dutch Colonial</t>
+  </si>
+  <si>
+    <t>Fortification | Colonial Spanish American</t>
+  </si>
+  <si>
+    <t>South America--Rio Negro | Guyana</t>
+  </si>
+  <si>
+    <t>Guyana--Essequibo</t>
+  </si>
+  <si>
+    <t>Brazil--Santarém (Pará)</t>
+  </si>
+  <si>
+    <t>Brazil--Macapá (Amapá)</t>
+  </si>
+  <si>
+    <t>Brazil--Gurupá (Pará)</t>
+  </si>
+  <si>
+    <t>1616-01-01</t>
+  </si>
+  <si>
+    <t>1776-12-31</t>
+  </si>
+  <si>
+    <t>Direct link via BNDigital @ http://objdigital.bn.br/objdigital2/acervo_digital/div_manuscritos/mss1456658/mss1456658.pdf</t>
+  </si>
+  <si>
+    <t>Direct link via fortalezas.org @ http://fortalezas.org/index.php?ct=fortaleza&amp;id_fortaleza=394</t>
+  </si>
+  <si>
+    <t>Source @ http://mw2.google.com/mw-panoramio/photos/medium/51797568.jpg</t>
+  </si>
+  <si>
+    <t>Direct link via fortalezas.org @ http://fortalezas.org/index.php?ct=fortaleza&amp;id_fortaleza=46</t>
+  </si>
+  <si>
+    <t>Direct link via fortalezas.org @ http://fortalezas.org/index.php?ct=fortaleza&amp;id_fortaleza=34</t>
+  </si>
+  <si>
+    <t>Direct link via fortalezas.org @ http://fortalezas.org/index.php?ct=fortaleza&amp;id_fortaleza=213</t>
+  </si>
+  <si>
+    <t>More information via Atlas of Mutual Heritage @ http://www.atlasofmutualheritage.nl/nl/Kyk-Overal.1063p</t>
+  </si>
+  <si>
+    <t>More information at UNESCO @ http://whc.unesco.org/en/tentativelists/273/</t>
+  </si>
+  <si>
+    <t>Source via JSTOR @ http://www.jstor.org/stable/10.2307/978188?ref=search- gateway:46ccfc6689b4c9d762dbc0a6aaef6ab9</t>
+  </si>
+  <si>
+    <t>Direct link via fortalezas.org @ http://fortalezas.org/?ct=fortaleza&amp;id_fortaleza=205</t>
+  </si>
+  <si>
+    <t>1500-01-01</t>
+  </si>
+  <si>
+    <t>1800-12-31</t>
+  </si>
+  <si>
+    <t>1766-12-31</t>
+  </si>
+  <si>
+    <t>1697-12-31</t>
+  </si>
+  <si>
+    <t>1616-12-31</t>
+  </si>
+  <si>
+    <t>1734-12-31</t>
+  </si>
+  <si>
+    <t>1624-12-31</t>
+  </si>
+  <si>
+    <t>1776, June Construction Started</t>
+  </si>
+  <si>
+    <t>1776-01-01</t>
+  </si>
+  <si>
+    <t>1781-12-31</t>
+  </si>
+  <si>
+    <t>1623-12-31</t>
+  </si>
+  <si>
+    <t>1764-01-02</t>
+  </si>
+  <si>
+    <t>1766-01-01</t>
+  </si>
+  <si>
+    <t>1697-01-01</t>
+  </si>
+  <si>
+    <t>1734-01-01</t>
+  </si>
+  <si>
+    <t>1754-01-01</t>
+  </si>
+  <si>
+    <t>1764-12-31</t>
+  </si>
+  <si>
+    <t>1700-01-01</t>
+  </si>
+  <si>
+    <t>1799-12-31</t>
+  </si>
+  <si>
+    <t>1609-01-01</t>
+  </si>
+  <si>
+    <t>Forte Do Castelo Do Senhor Santo Cristo Do Presépio De Belém.tiff</t>
+  </si>
+  <si>
+    <t>Forte do Presépio (Praça Frei Caetano Brandão) Belém Established 1616.kmz</t>
+  </si>
+  <si>
+    <t>Fortalezza de São José do Macapá.tiff</t>
+  </si>
+  <si>
+    <t>Fortalezza de São José do Macapá.kmz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Forte da São Francisco Xavier de Tabatinga.tiff</t>
+  </si>
+  <si>
+    <t>Forte da São Francisco Xavier de Tabatinga (1766).kmz</t>
+  </si>
+  <si>
+    <t>Forte Dos Tapajós (Santarém) .tiff</t>
+  </si>
+  <si>
+    <t>Forte Dos Tapajós (Santarém).kmz</t>
+  </si>
+  <si>
+    <t>Fort Island- Kyk Overal (Dutch Fort).tiff</t>
+  </si>
+  <si>
+    <t>Fort Island Kyk Overal (Dutch Fort).kmz</t>
+  </si>
+  <si>
+    <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island).tiff</t>
+  </si>
+  <si>
+    <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island).kmz</t>
+  </si>
+  <si>
+    <t>Fort San Carlos de Río Negro (Exact Location Unknown).tiff</t>
+  </si>
+  <si>
+    <t>Fort San Carlos de Río Negro (Exact Location Unknown).kmz</t>
+  </si>
+  <si>
+    <t>Fort San Agustín  Rio Negro (Spanish Fort) Location Unknown (_).tiff</t>
+  </si>
+  <si>
+    <t>Fort San Agustin  Rio Negro (Spanish Fort) Location Unknown ().kmz</t>
+  </si>
+  <si>
+    <t>Santo Antônio do Gurupá (Founded as Mariocai by the Dutch).tiff</t>
+  </si>
+  <si>
+    <t>Santo Antônio do Gurupá (Founded as Mariocai by the Dutch).kmz</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +3061,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2878,12 +3093,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2892,6 +3101,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2946,7 +3160,313 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC0D494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFACD575"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3292,674 +3812,1439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="48" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" customWidth="1"/>
     <col min="7" max="7" width="51.5703125" style="3" customWidth="1"/>
     <col min="8" max="9" width="45.140625" style="3" customWidth="1"/>
-    <col min="10" max="11" width="45.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
     <col min="14" max="15" width="39.140625" style="3" customWidth="1"/>
     <col min="16" max="16" width="42.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="84.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="38.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="110.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="24" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>517</v>
-      </c>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>487</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="25" t="s">
         <v>450</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>520</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="R1" s="16" t="s">
+      <c r="O1" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>623</v>
+      </c>
+      <c r="S1" s="25" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>631</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>632</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S2" s="20"/>
+    </row>
+    <row r="3" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
+        <v>657</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21" t="s">
+        <v>685</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
+        <v>682</v>
+      </c>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21" t="s">
+        <v>693</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>694</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>633</v>
+      </c>
+      <c r="S3" s="21"/>
+    </row>
+    <row r="4" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>659</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>658</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>683</v>
       </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-    </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="I4" s="20"/>
+      <c r="J4" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>646</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>485</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-    </row>
-    <row r="4" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>633</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>684</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>691</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21" t="s">
+        <v>718</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>719</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>666</v>
+      </c>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>646</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>660</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>661</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+    </row>
+    <row r="7" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>646</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>663</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21" t="s">
+        <v>662</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+    </row>
+    <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>384</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>658</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-    </row>
-    <row r="5" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>646</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20" t="s">
+        <v>725</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>726</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S8" s="20" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>664</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>661</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+    </row>
+    <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>665</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
+        <v>662</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+    </row>
+    <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
+        <v>639</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R11" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23" t="s">
-        <v>666</v>
-      </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-    </row>
-    <row r="6" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>646</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="S11" s="20" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>660</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="C12" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E12" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23" t="s">
-        <v>661</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-    </row>
-    <row r="7" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>646</v>
-      </c>
-      <c r="B7" s="23" t="s">
+      <c r="F12" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+    </row>
+    <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>663</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="C13" s="20" t="s">
+        <v>739</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23" t="s">
-        <v>662</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-    </row>
-    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>647</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+    </row>
+    <row r="14" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>649</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22" t="s">
-        <v>642</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
-        <v>667</v>
-      </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-    </row>
-    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>647</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20" t="s">
+        <v>674</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="Q14" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R14" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S14" s="20" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>649</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>664</v>
-      </c>
-      <c r="D9" s="22" t="s">
+      <c r="C15" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F15" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>661</v>
-      </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-    </row>
-    <row r="10" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>647</v>
-      </c>
-      <c r="B10" s="22" t="s">
+      <c r="G15" s="20"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+    </row>
+    <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>649</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C16" s="20" t="s">
+        <v>741</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-    </row>
-    <row r="11" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>648</v>
-      </c>
-      <c r="B11" s="22" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+    </row>
+    <row r="17" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22" t="s">
-        <v>639</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22" t="s">
-        <v>674</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22" t="s">
-        <v>668</v>
-      </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-    </row>
-    <row r="12" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>649</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
+        <v>638</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>720</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R17" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S17" s="20" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+    </row>
+    <row r="19" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>743</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+    </row>
+    <row r="20" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22" t="s">
-        <v>637</v>
-      </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22" t="s">
-        <v>675</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22" t="s">
-        <v>669</v>
-      </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-    </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>650</v>
-      </c>
-      <c r="B13" s="22" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
+        <v>640</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20" t="s">
+        <v>676</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>721</v>
+      </c>
+      <c r="N20" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q20" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R20" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S20" s="20" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+    </row>
+    <row r="22" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>745</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+    </row>
+    <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22" t="s">
-        <v>638</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22" t="s">
-        <v>670</v>
-      </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-    </row>
-    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>651</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L23" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="M23" s="20" t="s">
+        <v>722</v>
+      </c>
+      <c r="N23" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q23" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="R23" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S23" s="20" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+    </row>
+    <row r="25" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+    </row>
+    <row r="26" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22" t="s">
-        <v>677</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22" t="s">
-        <v>671</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-    </row>
-    <row r="15" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20" t="s">
+        <v>643</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>732</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="N26" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q26" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="R26" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+    </row>
+    <row r="28" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+    </row>
+    <row r="29" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22" t="s">
-        <v>634</v>
-      </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22" t="s">
-        <v>678</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22" t="s">
-        <v>672</v>
-      </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-    </row>
-    <row r="16" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="B16" s="22" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>686</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>679</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>733</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q29" s="20" t="s">
+        <v>700</v>
+      </c>
+      <c r="R29" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S29" s="20" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>750</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+    </row>
+    <row r="31" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+    </row>
+    <row r="32" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22" t="s">
-        <v>643</v>
-      </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22" t="s">
-        <v>679</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22" t="s">
-        <v>673</v>
-      </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-    </row>
-    <row r="17" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>654</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>686</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>735</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q32" s="20" t="s">
+        <v>700</v>
+      </c>
+      <c r="R32" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S32" s="20" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>752</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G33" s="20"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+    </row>
+    <row r="34" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>753</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+    </row>
+    <row r="35" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22" t="s">
-        <v>636</v>
-      </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22" t="s">
-        <v>680</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-    </row>
-    <row r="18" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22" t="s">
-        <v>635</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20" t="s">
+        <v>641</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20" t="s">
         <v>681</v>
       </c>
-      <c r="K18" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-    </row>
-    <row r="19" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="K35" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="L35" s="20" t="s">
+        <v>737</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q35" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="R35" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S35" s="20" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
         <v>656</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22" t="s">
-        <v>641</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22" t="s">
-        <v>682</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
+      <c r="B36" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>754</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>755</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>473</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="    \Sub-component">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="    \Sub-component">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="  \Component">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="  \Component">
       <formula>NOT(ISERROR(SEARCH("  \Component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Object">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Object">
       <formula>NOT(ISERROR(SEARCH("Object",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="    \Sub-component">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
   </dataValidations>
@@ -3968,7 +5253,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -3991,19 +5276,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>P1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q1</xm:sqref>
+          <xm:sqref>P1:R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>R1</xm:sqref>
+          <xm:sqref>S1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -4015,13 +5294,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>N1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>O1</xm:sqref>
+          <xm:sqref>N1:O1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
@@ -4119,7 +5392,7 @@
       <c r="F2" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>508</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -4235,7 +5508,7 @@
       <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>624</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -4261,7 +5534,7 @@
       <c r="F7" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="18" t="s">
         <v>621</v>
       </c>
       <c r="H7" s="12" t="s">
@@ -4299,7 +5572,7 @@
       <c r="C9" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>626</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -4341,13 +5614,13 @@
       <c r="C11" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>627</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="18" t="s">
         <v>622</v>
       </c>
       <c r="H11" s="11"/>
@@ -4425,7 +5698,7 @@
       <c r="F15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="18" t="s">
         <v>623</v>
       </c>
     </row>
@@ -4570,7 +5843,7 @@
       <c r="C26" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>628</v>
       </c>
     </row>
@@ -4603,7 +5876,7 @@
       <c r="C29" s="14" t="s">
         <v>543</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>625</v>
       </c>
     </row>
@@ -4677,7 +5950,7 @@
       <c r="C36" s="14" t="s">
         <v>546</v>
       </c>
-      <c r="E36" s="19"/>
+      <c r="E36" s="17"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
@@ -4686,7 +5959,7 @@
       <c r="C37" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
@@ -4695,7 +5968,7 @@
       <c r="C38" s="14" t="s">
         <v>547</v>
       </c>
-      <c r="E38" s="18"/>
+      <c r="E38" s="16"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">

</xml_diff>

<commit_message>
Added project for HLHW one offs, also tweaked Amazonia OLR for another test ingest
</commit_message>
<xml_diff>
--- a/amazonia/OLR/xls_standard_input_amazonia.xlsx
+++ b/amazonia/OLR/xls_standard_input_amazonia.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="737">
   <si>
     <t>text</t>
   </si>
@@ -2069,12 +2069,6 @@
     <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island)</t>
   </si>
   <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
     <t>0004</t>
   </si>
   <si>
@@ -2108,15 +2102,6 @@
     <t>0014</t>
   </si>
   <si>
-    <t xml:space="preserve">Forte de Tabatinga (Now in Brazil) - </t>
-  </si>
-  <si>
-    <t>Diário da viagem filosófica pela capitania de São José do Rio Negro; com a informação do estado presente dos estabelecimentos portugueses na sobredita Capitania, desde a vila capital de Barcelos até a fortaleza da barra do dito rio</t>
-  </si>
-  <si>
-    <t>Diario de viagem filosofica pela capitania de sao jose do rio negro.pdf</t>
-  </si>
-  <si>
     <t>Colonial Era Forts.tiff</t>
   </si>
   <si>
@@ -2126,13 +2111,7 @@
     <t>Mapping File</t>
   </si>
   <si>
-    <t>Colonial Era Forts.kmz</t>
-  </si>
-  <si>
     <t>Real Forte Príncipe da Beira.tiff</t>
-  </si>
-  <si>
-    <t>Real Forte Príncipe da Beira.kmz</t>
   </si>
   <si>
     <t>Complete Section Map</t>
@@ -2210,13 +2189,7 @@
     <t>2016</t>
   </si>
   <si>
-    <t>Ferreira, Alexandre Rodrigues, 1756-1815</t>
-  </si>
-  <si>
     <t>Deavenport, James</t>
-  </si>
-  <si>
-    <t>Archivo General de la Nación de Colombia</t>
   </si>
   <si>
     <t>Smith, Robert C.</t>
@@ -2240,18 +2213,12 @@
 http://www.atlasofmutualheritage.nl/nl/Zeelandia-fort-Essequibo.255c</t>
   </si>
   <si>
-    <t>1786</t>
-  </si>
-  <si>
     <t>~ 1500 - 1800</t>
   </si>
   <si>
     <t>1616-1776</t>
   </si>
   <si>
-    <t>Photographs Taken by James Deavenport, 2015</t>
-  </si>
-  <si>
     <t>Fortification</t>
   </si>
   <si>
@@ -2294,9 +2261,6 @@
     <t>1776-12-31</t>
   </si>
   <si>
-    <t>Direct link via BNDigital @ http://objdigital.bn.br/objdigital2/acervo_digital/div_manuscritos/mss1456658/mss1456658.pdf</t>
-  </si>
-  <si>
     <t>Direct link via fortalezas.org @ http://fortalezas.org/index.php?ct=fortaleza&amp;id_fortaleza=394</t>
   </si>
   <si>
@@ -2387,55 +2351,34 @@
     <t>Forte Do Castelo Do Senhor Santo Cristo Do Presépio De Belém.tiff</t>
   </si>
   <si>
-    <t>Forte do Presépio (Praça Frei Caetano Brandão) Belém Established 1616.kmz</t>
-  </si>
-  <si>
     <t>Fortalezza de São José do Macapá.tiff</t>
   </si>
   <si>
-    <t>Fortalezza de São José do Macapá.kmz</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Forte da São Francisco Xavier de Tabatinga.tiff</t>
   </si>
   <si>
-    <t>Forte da São Francisco Xavier de Tabatinga (1766).kmz</t>
-  </si>
-  <si>
     <t>Forte Dos Tapajós (Santarém) .tiff</t>
   </si>
   <si>
-    <t>Forte Dos Tapajós (Santarém).kmz</t>
-  </si>
-  <si>
-    <t>Fort Island- Kyk Overal (Dutch Fort).tiff</t>
-  </si>
-  <si>
-    <t>Fort Island Kyk Overal (Dutch Fort).kmz</t>
-  </si>
-  <si>
     <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island).tiff</t>
   </si>
   <si>
-    <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island).kmz</t>
-  </si>
-  <si>
     <t>Fort San Carlos de Río Negro (Exact Location Unknown).tiff</t>
   </si>
   <si>
-    <t>Fort San Carlos de Río Negro (Exact Location Unknown).kmz</t>
-  </si>
-  <si>
     <t>Fort San Agustín  Rio Negro (Spanish Fort) Location Unknown (_).tiff</t>
   </si>
   <si>
-    <t>Fort San Agustin  Rio Negro (Spanish Fort) Location Unknown ().kmz</t>
-  </si>
-  <si>
     <t>Santo Antônio do Gurupá (Founded as Mariocai by the Dutch).tiff</t>
   </si>
   <si>
-    <t>Santo Antônio do Gurupá (Founded as Mariocai by the Dutch).kmz</t>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Colonial Era Forts info.zip</t>
+  </si>
+  <si>
+    <t>Fort Island_ Kyk Overal (Dutch Fort).tiff</t>
   </si>
 </sst>
 </file>
@@ -3061,7 +3004,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3106,6 +3049,7 @@
     </xf>
     <xf numFmtId="49" fontId="28" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3160,313 +3104,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -3812,18 +3450,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C37" sqref="C37"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="60.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="73.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" customWidth="1"/>
@@ -3903,7 +3541,7 @@
       <c r="A2" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="26" t="s">
         <v>485</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -3922,22 +3560,22 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="20" t="s">
-        <v>694</v>
+        <v>683</v>
       </c>
       <c r="R2" s="20" t="s">
         <v>633</v>
@@ -3948,7 +3586,7 @@
       <c r="A3" s="21" t="s">
         <v>644</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="26" t="s">
         <v>485</v>
       </c>
       <c r="C3" s="21"/>
@@ -3956,192 +3594,190 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21" t="s">
-        <v>657</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
-        <v>685</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
-        <v>682</v>
-      </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21" t="s">
-        <v>693</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>696</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>694</v>
-      </c>
-      <c r="R3" s="21" t="s">
         <v>633</v>
       </c>
+      <c r="H3" s="21" t="s">
+        <v>676</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
+        <v>681</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
+        <v>706</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>659</v>
+      </c>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>633</v>
+      </c>
       <c r="S3" s="21"/>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>645</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>659</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>658</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>683</v>
-      </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>708</v>
-      </c>
+    <row r="4" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>655</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>656</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
     </row>
     <row r="5" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>646</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>485</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+        <v>644</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>735</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>473</v>
+      </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>633</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>684</v>
-      </c>
+        <v>657</v>
+      </c>
+      <c r="H5" s="21"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="21" t="s">
-        <v>691</v>
-      </c>
+      <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="21" t="s">
-        <v>718</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>719</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>666</v>
-      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
-      <c r="Q5" s="20" t="s">
-        <v>694</v>
-      </c>
-      <c r="R5" s="20" t="s">
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>676</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>715</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>660</v>
+      </c>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R6" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="S5" s="21"/>
-    </row>
-    <row r="6" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>646</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>524</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>660</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="S6" s="20" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>658</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>661</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-    </row>
-    <row r="7" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>646</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>524</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>663</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>473</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21" t="s">
-        <v>662</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
+      <c r="G7" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="B8" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>485</v>
       </c>
       <c r="C8" s="20"/>
@@ -4149,50 +3785,50 @@
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>725</v>
+        <v>666</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>726</v>
+        <v>695</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="R8" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>709</v>
+        <v>698</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>524</v>
+        <v>646</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>734</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>664</v>
+        <v>726</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>359</v>
@@ -4203,9 +3839,7 @@
       <c r="F9" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>661</v>
-      </c>
+      <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -4223,134 +3857,150 @@
       <c r="A10" s="20" t="s">
         <v>647</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>473</v>
-      </c>
+      <c r="B10" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="N10" s="20" t="s">
         <v>662</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
       <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
+      <c r="P10" s="20" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S10" s="20" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>639</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>684</v>
-      </c>
+        <v>647</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>706</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>728</v>
-      </c>
-      <c r="N11" s="20" t="s">
-        <v>668</v>
-      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="20"/>
-      <c r="P11" s="20" t="s">
-        <v>695</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>698</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S11" s="20" t="s">
-        <v>710</v>
-      </c>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
     </row>
     <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>738</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="B12" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>638</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>676</v>
+      </c>
       <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="J12" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>663</v>
+      </c>
       <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
+      <c r="P12" s="20" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q12" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R12" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S12" s="20" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>524</v>
+      <c r="B13" s="26" t="s">
+        <v>734</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>403</v>
+        <v>359</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F13" s="20"/>
+        <v>341</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -4367,7 +4017,7 @@
       <c r="A14" s="20" t="s">
         <v>649</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="26" t="s">
         <v>485</v>
       </c>
       <c r="C14" s="20"/>
@@ -4375,50 +4025,50 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="I14" s="20"/>
       <c r="J14" s="20" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>729</v>
+        <v>709</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="O14" s="20"/>
       <c r="P14" s="20" t="s">
-        <v>704</v>
+        <v>692</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="R14" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>711</v>
+        <v>701</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>649</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>524</v>
+      <c r="B15" s="26" t="s">
+        <v>734</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>359</v>
@@ -4445,132 +4095,154 @@
     </row>
     <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>649</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>741</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>473</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>665</v>
+      </c>
       <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
+      <c r="P16" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q16" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="R16" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S16" s="20" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="17" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
-        <v>638</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>684</v>
-      </c>
+      <c r="B17" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>736</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="23"/>
       <c r="I17" s="20"/>
-      <c r="J17" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>730</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>720</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>670</v>
-      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="20" t="s">
-        <v>696</v>
-      </c>
-      <c r="Q17" s="20" t="s">
-        <v>698</v>
-      </c>
-      <c r="R17" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S17" s="20" t="s">
-        <v>712</v>
-      </c>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
     </row>
     <row r="18" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>742</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+        <v>651</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>643</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>679</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>720</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>711</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>680</v>
+      </c>
       <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="P18" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S18" s="20" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="19" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>743</v>
+        <v>651</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>730</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>403</v>
+        <v>359</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F19" s="20"/>
+        <v>341</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G19" s="20"/>
       <c r="H19" s="23"/>
       <c r="I19" s="20"/>
@@ -4587,9 +4259,9 @@
     </row>
     <row r="20" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="B20" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>485</v>
       </c>
       <c r="C20" s="20"/>
@@ -4597,50 +4269,50 @@
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I20" s="20"/>
+        <v>676</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>677</v>
+      </c>
       <c r="J20" s="20" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>721</v>
-      </c>
-      <c r="N20" s="20" t="s">
-        <v>671</v>
-      </c>
+        <v>722</v>
+      </c>
+      <c r="N20" s="20"/>
       <c r="O20" s="20"/>
       <c r="P20" s="20" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="R20" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S20" s="20" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>744</v>
+        <v>652</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>359</v>
@@ -4667,580 +4339,164 @@
     </row>
     <row r="22" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>745</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>473</v>
-      </c>
+        <v>653</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
+      <c r="G22" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>724</v>
+      </c>
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
+      <c r="P22" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="R22" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S22" s="20" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20" t="s">
-        <v>634</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>687</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>677</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L23" s="20" t="s">
-        <v>706</v>
-      </c>
-      <c r="M23" s="20" t="s">
-        <v>722</v>
-      </c>
-      <c r="N23" s="20" t="s">
-        <v>672</v>
-      </c>
+        <v>653</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
       <c r="O23" s="20"/>
-      <c r="P23" s="20" t="s">
-        <v>702</v>
-      </c>
-      <c r="Q23" s="20" t="s">
-        <v>699</v>
-      </c>
-      <c r="R23" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S23" s="20" t="s">
-        <v>714</v>
-      </c>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
     </row>
     <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>746</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="23"/>
+        <v>654</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20" t="s">
+        <v>641</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>676</v>
+      </c>
       <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
+      <c r="J24" s="20" t="s">
+        <v>674</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>725</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>712</v>
+      </c>
       <c r="N24" s="20"/>
       <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-    </row>
-    <row r="25" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q24" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R24" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S24" s="20" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>524</v>
+        <v>654</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>734</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>403</v>
+        <v>359</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-    </row>
-    <row r="26" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>688</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="K26" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>732</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>723</v>
-      </c>
-      <c r="N26" s="20" t="s">
-        <v>689</v>
-      </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20" t="s">
-        <v>702</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>699</v>
-      </c>
-      <c r="R26" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S26" s="20" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E27" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F25" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-    </row>
-    <row r="28" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>749</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-    </row>
-    <row r="29" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>686</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>679</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L29" s="20" t="s">
-        <v>733</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>734</v>
-      </c>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20" t="s">
-        <v>701</v>
-      </c>
-      <c r="Q29" s="20" t="s">
-        <v>700</v>
-      </c>
-      <c r="R29" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S29" s="20" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>750</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-    </row>
-    <row r="31" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>751</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-    </row>
-    <row r="32" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>686</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L32" s="20" t="s">
-        <v>735</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>736</v>
-      </c>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20" t="s">
-        <v>701</v>
-      </c>
-      <c r="Q32" s="20" t="s">
-        <v>700</v>
-      </c>
-      <c r="R32" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S32" s="20" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>752</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-    </row>
-    <row r="34" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>753</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-    </row>
-    <row r="35" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20" t="s">
-        <v>641</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>684</v>
-      </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20" t="s">
-        <v>681</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="L35" s="20" t="s">
-        <v>737</v>
-      </c>
-      <c r="M35" s="20" t="s">
-        <v>724</v>
-      </c>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20" t="s">
-        <v>705</v>
-      </c>
-      <c r="Q35" s="20" t="s">
-        <v>698</v>
-      </c>
-      <c r="R35" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S35" s="20" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>755</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>473</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="    \Sub-component">
+  <conditionalFormatting sqref="B1 B26:B1048576">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="    \Sub-component">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="  \Component">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="  \Component">
       <formula>NOT(ISERROR(SEARCH("  \Component",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Object">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="Object">
       <formula>NOT(ISERROR(SEARCH("Object",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="    \Sub-component">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5298,6 +4554,12 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
+            <xm:f>'CV values'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B26:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
+          <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
@@ -5307,12 +4569,6 @@
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
-          <x14:formula1>
-            <xm:f>'CV values'!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>

<commit_message>
Removed components that only had one file, made into objects
</commit_message>
<xml_diff>
--- a/amazonia/OLR/xls_standard_input_amazonia.xlsx
+++ b/amazonia/OLR/xls_standard_input_amazonia.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="737">
   <si>
     <t>text</t>
   </si>
@@ -3450,11 +3450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+      <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,10 +3698,18 @@
       <c r="B6" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>658</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>642</v>
       </c>
@@ -3740,13 +3748,13 @@
     </row>
     <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>734</v>
+        <v>485</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>658</v>
+        <v>726</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>359</v>
@@ -3758,57 +3766,85 @@
         <v>361</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="H7" s="20"/>
+        <v>639</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>676</v>
+      </c>
       <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="20" t="s">
+        <v>666</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>661</v>
+      </c>
       <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
+      <c r="P7" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="C8" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G8" s="20" t="s">
-        <v>639</v>
-      </c>
-      <c r="H8" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>676</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>675</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>695</v>
+        <v>717</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="Q8" s="20" t="s">
         <v>687</v>
@@ -3817,18 +3853,18 @@
         <v>633</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>734</v>
+        <v>485</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>359</v>
@@ -3839,56 +3875,86 @@
       <c r="F9" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="G9" s="20" t="s">
+        <v>638</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>676</v>
+      </c>
       <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>663</v>
+      </c>
       <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
+      <c r="P9" s="20" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S9" s="20" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G10" s="20" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="H10" s="23" t="s">
         <v>676</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="K10" s="20" t="s">
         <v>675</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="20" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="Q10" s="20" t="s">
         <v>687</v>
@@ -3897,18 +3963,18 @@
         <v>633</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>727</v>
+        <v>485</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>736</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>359</v>
@@ -3919,76 +3985,110 @@
       <c r="F11" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="G11" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>665</v>
+      </c>
       <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
+      <c r="P11" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S11" s="20" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G12" s="20" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="H12" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="20" t="s">
+        <v>679</v>
+      </c>
       <c r="J12" s="20" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="K12" s="20" t="s">
         <v>675</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>663</v>
+        <v>680</v>
       </c>
       <c r="O12" s="20"/>
       <c r="P12" s="20" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="Q12" s="20" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="R12" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S12" s="20" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>728</v>
+        <v>485</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>359</v>
@@ -3999,76 +4099,106 @@
       <c r="F13" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>676</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>721</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>722</v>
+      </c>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
+      <c r="P13" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q13" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="14" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="C14" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G14" s="20" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="I14" s="20"/>
+      <c r="I14" s="20" t="s">
+        <v>677</v>
+      </c>
       <c r="J14" s="20" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>675</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>709</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>664</v>
-      </c>
+        <v>724</v>
+      </c>
+      <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="20" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="R14" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>729</v>
+        <v>485</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>733</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>359</v>
@@ -4079,411 +4209,42 @@
       <c r="F15" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="20" t="s">
+        <v>641</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>676</v>
+      </c>
       <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
+      <c r="J15" s="20" t="s">
+        <v>674</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>725</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>712</v>
+      </c>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-    </row>
-    <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20" t="s">
-        <v>634</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>670</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>695</v>
-      </c>
-      <c r="M16" s="20" t="s">
-        <v>710</v>
-      </c>
-      <c r="N16" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20" t="s">
-        <v>691</v>
-      </c>
-      <c r="Q16" s="20" t="s">
-        <v>688</v>
-      </c>
-      <c r="R16" s="20" t="s">
+      <c r="P15" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q15" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="R15" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="S16" s="20" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>736</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-    </row>
-    <row r="18" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>679</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="K18" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L18" s="20" t="s">
-        <v>720</v>
-      </c>
-      <c r="M18" s="20" t="s">
-        <v>711</v>
-      </c>
-      <c r="N18" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20" t="s">
-        <v>691</v>
-      </c>
-      <c r="Q18" s="20" t="s">
-        <v>688</v>
-      </c>
-      <c r="R18" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S18" s="20" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>730</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-    </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>677</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>672</v>
-      </c>
-      <c r="K20" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>721</v>
-      </c>
-      <c r="M20" s="20" t="s">
-        <v>722</v>
-      </c>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="Q20" s="20" t="s">
-        <v>689</v>
-      </c>
-      <c r="R20" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S20" s="20" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>731</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-    </row>
-    <row r="22" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>677</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>723</v>
-      </c>
-      <c r="M22" s="20" t="s">
-        <v>724</v>
-      </c>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>689</v>
-      </c>
-      <c r="R22" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S22" s="20" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>653</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>732</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-    </row>
-    <row r="24" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20" t="s">
-        <v>641</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20" t="s">
-        <v>674</v>
-      </c>
-      <c r="K24" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>725</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>712</v>
-      </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20" t="s">
-        <v>694</v>
-      </c>
-      <c r="Q24" s="20" t="s">
-        <v>687</v>
-      </c>
-      <c r="R24" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S24" s="20" t="s">
+      <c r="S15" s="20" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>733</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>361</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B26:B1048576">
+  <conditionalFormatting sqref="B1 B16:B1048576">
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
@@ -4556,25 +4317,25 @@
           <x14:formula1>
             <xm:f>'CV values'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B26:B1048576</xm:sqref>
+          <xm:sqref>B16:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D15 D16:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E2:E15 E16:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F15 F16:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adjusted wrangling from input at meeting
</commit_message>
<xml_diff>
--- a/amazonia/OLR/xls_standard_input_amazonia.xlsx
+++ b/amazonia/OLR/xls_standard_input_amazonia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="339"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="8535" tabRatio="339"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="732">
   <si>
     <t>text</t>
   </si>
@@ -2067,9 +2067,6 @@
   </si>
   <si>
     <t>Zeelandia, Fort Essequibo (Dutch Fort on Flag Island)</t>
-  </si>
-  <si>
-    <t>0004</t>
   </si>
   <si>
     <t>0005</t>
@@ -2190,9 +2187,6 @@
   </si>
   <si>
     <t>Deavenport, James</t>
-  </si>
-  <si>
-    <t>Smith, Robert C.</t>
   </si>
   <si>
     <t>Sweet, David Graham</t>
@@ -2213,9 +2207,6 @@
 http://www.atlasofmutualheritage.nl/nl/Zeelandia-fort-Essequibo.255c</t>
   </si>
   <si>
-    <t>~ 1500 - 1800</t>
-  </si>
-  <si>
     <t>1616-1776</t>
   </si>
   <si>
@@ -2288,12 +2279,6 @@
     <t>Direct link via fortalezas.org @ http://fortalezas.org/?ct=fortaleza&amp;id_fortaleza=205</t>
   </si>
   <si>
-    <t>1500-01-01</t>
-  </si>
-  <si>
-    <t>1800-12-31</t>
-  </si>
-  <si>
     <t>1766-12-31</t>
   </si>
   <si>
@@ -2375,10 +2360,10 @@
     <t>Component</t>
   </si>
   <si>
-    <t>Colonial Era Forts info.zip</t>
-  </si>
-  <si>
     <t>Fort Island_ Kyk Overal (Dutch Fort).tiff</t>
+  </si>
+  <si>
+    <t>Deavenport, James | Smith, Robert C.</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +2989,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3042,8 +3027,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -3450,11 +3433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,61 +3462,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="23" t="s">
         <v>455</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="23" t="s">
         <v>460</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="23" t="s">
         <v>623</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="23" t="s">
         <v>483</v>
       </c>
     </row>
@@ -3541,11 +3524,8 @@
       <c r="A2" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>485</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>631</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>403</v>
@@ -3553,153 +3533,175 @@
       <c r="E2" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="F2" s="20"/>
+      <c r="F2" s="20" t="s">
+        <v>361</v>
+      </c>
       <c r="G2" s="20" t="s">
         <v>632</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" t="s">
+        <v>675</v>
+      </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>696</v>
-      </c>
-      <c r="N2" s="20"/>
+        <v>693</v>
+      </c>
+      <c r="N2" t="s">
+        <v>658</v>
+      </c>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="20" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="R2" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="B3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C3" t="s">
+        <v>654</v>
+      </c>
+      <c r="D3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G3" t="s">
+        <v>655</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="B4" t="s">
+        <v>729</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>631</v>
+      </c>
+      <c r="D4" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" t="s">
+        <v>473</v>
+      </c>
+      <c r="F4" t="s">
+        <v>361</v>
+      </c>
+      <c r="G4" t="s">
+        <v>656</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="C5" s="20" t="s">
+        <v>657</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>674</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>709</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>659</v>
+      </c>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="R5" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>676</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21" t="s">
-        <v>681</v>
-      </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21" t="s">
-        <v>706</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>707</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>659</v>
-      </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="20" t="s">
-        <v>683</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S3" s="21"/>
-    </row>
-    <row r="4" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>644</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>655</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>341</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>361</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>656</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-    </row>
-    <row r="5" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>644</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>734</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>735</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>473</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21" t="s">
-        <v>657</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
+      <c r="S5" s="20" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>645</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>485</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>658</v>
+        <v>721</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>359</v>
@@ -3711,50 +3713,50 @@
         <v>361</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20" t="s">
-        <v>713</v>
+        <v>665</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>660</v>
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="20" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="R6" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>646</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="24" t="s">
         <v>485</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>359</v>
@@ -3766,50 +3768,50 @@
         <v>361</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>639</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>676</v>
+        <v>637</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>675</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20" t="s">
         <v>666</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>695</v>
+        <v>712</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="N7" s="20" t="s">
         <v>661</v>
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q7" s="20" t="s">
         <v>684</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>687</v>
       </c>
       <c r="R7" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S7" s="20" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>647</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>485</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>359</v>
@@ -3821,50 +3823,50 @@
         <v>361</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>637</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>676</v>
+        <v>638</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>675</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
         <v>667</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="N8" s="20" t="s">
         <v>662</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>693</v>
+        <v>682</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="R8" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>485</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>359</v>
@@ -3876,50 +3878,50 @@
         <v>361</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>638</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>676</v>
+        <v>640</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>675</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
         <v>668</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="N9" s="20" t="s">
         <v>663</v>
       </c>
       <c r="O9" s="20"/>
       <c r="P9" s="20" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="R9" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>649</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>729</v>
+      <c r="C10" s="21" t="s">
+        <v>730</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>359</v>
@@ -3931,50 +3933,52 @@
         <v>361</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>640</v>
-      </c>
-      <c r="H10" s="23" t="s">
+        <v>634</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>675</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>676</v>
       </c>
-      <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
         <v>669</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>719</v>
+        <v>692</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="N10" s="20" t="s">
         <v>664</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="20" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="R10" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>736</v>
+      <c r="C11" s="21" t="s">
+        <v>725</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>359</v>
@@ -3986,52 +3990,52 @@
         <v>361</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>634</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>676</v>
+        <v>643</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>675</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>670</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>695</v>
+        <v>715</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>665</v>
+        <v>678</v>
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="20" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="R11" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S11" s="20" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>651</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>730</v>
+      <c r="C12" s="21" t="s">
+        <v>726</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>359</v>
@@ -4043,52 +4047,48 @@
         <v>361</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>679</v>
-      </c>
+        <v>636</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>731</v>
+      </c>
+      <c r="I12" s="20"/>
       <c r="J12" s="20" t="s">
         <v>671</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>711</v>
-      </c>
-      <c r="N12" s="20" t="s">
-        <v>680</v>
-      </c>
+        <v>717</v>
+      </c>
+      <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="Q12" s="20" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="R12" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S12" s="20" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>652</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>731</v>
+      <c r="C13" s="21" t="s">
+        <v>727</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>359</v>
@@ -4100,50 +4100,48 @@
         <v>361</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>677</v>
-      </c>
+        <v>635</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>731</v>
+      </c>
+      <c r="I13" s="20"/>
       <c r="J13" s="20" t="s">
         <v>672</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="R13" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S13" s="20" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>653</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>732</v>
+      <c r="C14" s="21" t="s">
+        <v>728</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>359</v>
@@ -4155,96 +4153,41 @@
         <v>361</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>677</v>
-      </c>
+        <v>641</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>675</v>
+      </c>
+      <c r="I14" s="20"/>
       <c r="J14" s="20" t="s">
         <v>673</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>724</v>
+        <v>707</v>
       </c>
       <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="20" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="R14" s="20" t="s">
         <v>633</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>733</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>641</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20" t="s">
-        <v>674</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="L15" s="20" t="s">
-        <v>725</v>
-      </c>
-      <c r="M15" s="20" t="s">
-        <v>712</v>
-      </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20" t="s">
-        <v>694</v>
-      </c>
-      <c r="Q15" s="20" t="s">
-        <v>687</v>
-      </c>
-      <c r="R15" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="S15" s="20" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B16:B1048576">
+  <conditionalFormatting sqref="B1 B15:B1048576">
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="    \Sub-component">
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
@@ -4261,7 +4204,7 @@
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
   </dataValidations>
@@ -4270,7 +4213,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -4317,25 +4260,25 @@
           <x14:formula1>
             <xm:f>'CV values'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B16:B1048576</xm:sqref>
+          <xm:sqref>B15:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D15 D16:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E15 E16:E1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F16:F1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>